<commit_message>
results updated to include safety
</commit_message>
<xml_diff>
--- a/outputs/UG_COnvid_jmmi_15may2020_safety reasons.xlsx
+++ b/outputs/UG_COnvid_jmmi_15may2020_safety reasons.xlsx
@@ -54,27 +54,27 @@
     <t xml:space="preserve">Relaxation of rules and regulations</t>
   </si>
   <si>
+    <t xml:space="preserve">Introduction of new rules and regulations</t>
+  </si>
+  <si>
     <t xml:space="preserve">No theft</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction of new rules and regulations</t>
-  </si>
-  <si>
     <t xml:space="preserve">n/a</t>
   </si>
   <si>
     <t xml:space="preserve">Installation of sanitary infrastructure</t>
   </si>
   <si>
+    <t xml:space="preserve">Appropriate behaviour of security personnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduced threats of disease spread</t>
+  </si>
+  <si>
     <t xml:space="preserve">No threats of covic infections</t>
   </si>
   <si>
-    <t xml:space="preserve">Appropriate behaviour of security personnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reduced threats of disease spread</t>
-  </si>
-  <si>
     <t xml:space="preserve">South West</t>
   </si>
   <si>
@@ -96,19 +96,19 @@
     <t xml:space="preserve">Fear of contracting COVID-19</t>
   </si>
   <si>
+    <t xml:space="preserve">Discretionary behaviour of security personnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health risks in relation to COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corona-infected individuals in the area</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fear of contracting COVID-20</t>
   </si>
   <si>
-    <t xml:space="preserve">Discretionary behaviour of security personnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health risks in relation to COVID-19</t>
-  </si>
-  <si>
     <t xml:space="preserve">Some people stopped working and may pose a big threat to our merchandise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corona-infected individuals in the area</t>
   </si>
   <si>
     <t xml:space="preserve">Lack of customers</t>
@@ -743,7 +743,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
         <v>0.111111111111111</v>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D19" t="n">
         <v>0.111111111111111</v>
@@ -777,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -862,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -896,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -964,7 +964,7 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" t="n">
         <v>0.0810810810810811</v>
@@ -981,7 +981,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D32" t="n">
         <v>0.0810810810810811</v>
@@ -998,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D33" t="n">
         <v>0.0540540540540541</v>
@@ -1015,7 +1015,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" t="n">
         <v>0.0540540540540541</v>
@@ -1032,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35" t="n">
         <v>0.027027027027027</v>
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" t="n">
         <v>0.027027027027027</v>
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D37" t="n">
         <v>0.027027027027027</v>
@@ -1083,7 +1083,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1117,7 +1117,7 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
@@ -1301,7 +1301,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1318,7 +1318,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -1335,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" t="n">
         <v>0.0909090909090909</v>
@@ -1403,7 +1403,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D16" t="n">
         <v>0.0909090909090909</v>
@@ -1420,7 +1420,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" t="n">
         <v>0.0909090909090909</v>
@@ -1437,7 +1437,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
         <v>0.0909090909090909</v>
@@ -1454,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1488,7 +1488,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1573,7 +1573,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" t="n">
         <v>0.1</v>
@@ -1590,7 +1590,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" t="n">
         <v>0.1</v>
@@ -1607,7 +1607,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28" t="n">
         <v>0.1</v>
@@ -1641,7 +1641,7 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -1658,7 +1658,7 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -1675,7 +1675,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -1709,7 +1709,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>

</xml_diff>